<commit_message>
adicionando formulas de soma e de multiplicação para validar o seguinte caso de uso. - após a planilha ter sido gerado o usuario poderá alterar os valores e a formula criada irá conseguir atualizar os campos sem aprentar erro
</commit_message>
<xml_diff>
--- a/src/main/resources/planilha-apache-poi.xlsx
+++ b/src/main/resources/planilha-apache-poi.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t xml:space="preserve">nome</t>
   </si>
@@ -45,6 +45,12 @@
   </si>
   <si>
     <t xml:space="preserve">LUCRO</t>
+  </si>
+  <si>
+    <t>VALOR</t>
+  </si>
+  <si>
+    <t>QUANTIDADE</t>
   </si>
 </sst>
 </file>
@@ -159,10 +165,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:G7"/>
+  <dimension ref="B2:G8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -186,7 +192,7 @@
       </c>
       <c r="G2" s="2" t="n">
         <f aca="false">Planilha2!D2</f>
-        <v>200.5</v>
+        <v>-30.0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -204,18 +210,39 @@
         <v>5</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>750.5</v>
+        <v>520.0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D5" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D6" s="0" t="n">
+        <v>500.3</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <f aca="false">SUM(D6:E6)</f>
+        <v>502.3</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <f aca="false">D6*E6</f>
+        <v>1000.6</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="1"/>
     </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:B7"/>
@@ -264,7 +291,7 @@
       </c>
       <c r="D2" s="0" t="n">
         <f aca="false">Planilha1!D4-C2</f>
-        <v>200.5</v>
+        <v>-30.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>